<commit_message>
global local sna metrics
</commit_message>
<xml_diff>
--- a/latex/thesis/others/SNA_metrics.xlsx
+++ b/latex/thesis/others/SNA_metrics.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b73f4100931222f3/WU/Semester 4/Thesis/git-miner/latex/thesis/others/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{0EE0E607-CBEF-488E-A6AA-9E8B1697CC16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{97F43439-355C-447E-8D69-9777D0BB2CE3}"/>
+  <xr:revisionPtr revIDLastSave="371" documentId="8_{0EE0E607-CBEF-488E-A6AA-9E8B1697CC16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8784BE00-F479-4209-9293-0F403763C715}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{4DF2AF1D-ED97-4676-8B35-8B544460FD2A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{4DF2AF1D-ED97-4676-8B35-8B544460FD2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$47</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="142">
   <si>
     <t>X</t>
   </si>
@@ -205,12 +209,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>no access</t>
-  </si>
-  <si>
-    <t>Access</t>
-  </si>
-  <si>
     <t>density, mean degree (avg and st dev), betweenness centrality, core/active developers</t>
   </si>
   <si>
@@ -281,14 +279,225 @@
   </si>
   <si>
     <t>!</t>
+  </si>
+  <si>
+    <t>connected components, weighted clustering coefficient</t>
+  </si>
+  <si>
+    <t>user follows</t>
+  </si>
+  <si>
+    <t>"we use Networkx to compute automatically SNA metrics for each graph."</t>
+  </si>
+  <si>
+    <t>files co-edition, committed comments, review's comments</t>
+  </si>
+  <si>
+    <t>not relevant, not network analysis</t>
+  </si>
+  <si>
+    <t>file-based (code collaboration)</t>
+  </si>
+  <si>
+    <t>eigenvector-centrality, degree-centrality, betweenness-centrality, network-density, cluster coeff., strength of ties</t>
+  </si>
+  <si>
+    <t>betweenness centrality</t>
+  </si>
+  <si>
+    <t>not social network</t>
+  </si>
+  <si>
+    <t>no social network</t>
+  </si>
+  <si>
+    <t>communication</t>
+  </si>
+  <si>
+    <t>developers vs used tools network</t>
+  </si>
+  <si>
+    <t>activity percentile</t>
+  </si>
+  <si>
+    <t>developer network</t>
+  </si>
+  <si>
+    <t>inter-project communities</t>
+  </si>
+  <si>
+    <t>Global Clustering Coefficient, Number of Nodes, Number of Ties (edges), Average Path Length (APL)</t>
+  </si>
+  <si>
+    <t>developer participation in projects</t>
+  </si>
+  <si>
+    <t>bug report</t>
+  </si>
+  <si>
+    <t>Degree of separation (dist), avg path length, Modularity, number of nodes</t>
+  </si>
+  <si>
+    <t>Betweenness Centrality,  Clustering Coefficient</t>
+  </si>
+  <si>
+    <t>Node count (size)</t>
+  </si>
+  <si>
+    <t>Network density</t>
+  </si>
+  <si>
+    <t>Number of components</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Brokerage roles</t>
+  </si>
+  <si>
+    <t>Proximity prestige</t>
+  </si>
+  <si>
+    <t>Ratio of core and active developers</t>
+  </si>
+  <si>
+    <t>Graph diameter</t>
+  </si>
+  <si>
+    <t>Clustering coefficient (weighted)</t>
+  </si>
+  <si>
+    <t>Strength of ties</t>
+  </si>
+  <si>
+    <t>Number of nodes</t>
+  </si>
+  <si>
+    <t>Global metrics</t>
+  </si>
+  <si>
+    <t>Local metrics</t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>Degree of a node</t>
+  </si>
+  <si>
+    <t>Aggregation</t>
+  </si>
+  <si>
+    <t>avg, st dev</t>
+  </si>
+  <si>
+    <t>How many edges there are compared to possible edge count</t>
+  </si>
+  <si>
+    <t>Component: nodes connected, that are not connected to any other node outside of the component</t>
+  </si>
+  <si>
+    <t>Number of K-cores</t>
+  </si>
+  <si>
+    <t>Number of components after removing nodes having a degree less than k</t>
+  </si>
+  <si>
+    <t>Inverse farness of a node to all other nodes</t>
+  </si>
+  <si>
+    <t>Number of shortest paths passing through the node</t>
+  </si>
+  <si>
+    <t>Measure of the degree to which nodes in a graph tend to cluster together</t>
+  </si>
+  <si>
+    <t>Ratio of number of core nodes versus the total number of nodes in the graph</t>
+  </si>
+  <si>
+    <t>The number of nodes in the "longest shortest path"</t>
+  </si>
+  <si>
+    <t>Path length</t>
+  </si>
+  <si>
+    <t>Number of nodes in the shortest path between two nodes</t>
+  </si>
+  <si>
+    <t>Preference for a network's nodes to attach to others that are similar in some way (nodes with degree of x tend to connect to other nodes also with degree of x)</t>
+  </si>
+  <si>
+    <t>Assortativity coefficient (aka degree correlation)</t>
+  </si>
+  <si>
+    <t>A high value means that a node is connected to many nodes who themselves have high scores.</t>
+  </si>
+  <si>
+    <t>Eigenvector centrality</t>
+  </si>
+  <si>
+    <t>Other metrics</t>
+  </si>
+  <si>
+    <t>Centralization</t>
+  </si>
+  <si>
+    <t>(Closeness centrality)</t>
+  </si>
+  <si>
+    <t>(Betweenness centrality)</t>
+  </si>
+  <si>
+    <t>Gini (measure of inequality) of the degrees OR in 2006 paper</t>
+  </si>
+  <si>
+    <t>Issues over time</t>
+  </si>
+  <si>
+    <t>lines added/deleted</t>
+  </si>
+  <si>
+    <t>commits over time</t>
+  </si>
+  <si>
+    <t>how long issues are open (?)</t>
+  </si>
+  <si>
+    <t>Convert Pathpy to networkx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -316,11 +525,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,10 +897,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40BE348-3A85-4F19-AC58-CEF0D458E489}">
-  <dimension ref="A1:L47"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,11 +909,11 @@
     <col min="1" max="1" width="96.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="7" width="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -719,19 +933,16 @@
         <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="K1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -744,14 +955,14 @@
       <c r="F2" t="s">
         <v>54</v>
       </c>
-      <c r="I2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -761,11 +972,8 @@
       <c r="F3" t="s">
         <v>55</v>
       </c>
-      <c r="G3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -776,19 +984,19 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
         <v>54</v>
       </c>
+      <c r="G4" t="s">
+        <v>59</v>
+      </c>
       <c r="H4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -796,19 +1004,19 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
         <v>54</v>
       </c>
+      <c r="G5" t="s">
+        <v>59</v>
+      </c>
       <c r="H5" t="s">
-        <v>61</v>
-      </c>
-      <c r="I5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -816,19 +1024,19 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
         <v>54</v>
       </c>
+      <c r="G6" t="s">
+        <v>59</v>
+      </c>
       <c r="H6" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -842,16 +1050,16 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F7" t="s">
         <v>54</v>
       </c>
-      <c r="I7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -859,16 +1067,16 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F8" t="s">
-        <v>67</v>
-      </c>
-      <c r="I8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="H8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -876,16 +1084,16 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
-      </c>
-      <c r="I9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="H9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -895,11 +1103,11 @@
       <c r="F10" t="s">
         <v>55</v>
       </c>
-      <c r="H10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
@@ -910,16 +1118,16 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
-      </c>
-      <c r="I11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="H11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -932,11 +1140,11 @@
       <c r="F12" t="s">
         <v>55</v>
       </c>
-      <c r="H12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -947,13 +1155,13 @@
         <v>55</v>
       </c>
       <c r="F13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="G13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -963,11 +1171,11 @@
       <c r="F14" t="s">
         <v>55</v>
       </c>
-      <c r="H14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -978,16 +1186,16 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F15" t="s">
         <v>54</v>
       </c>
-      <c r="I15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -998,19 +1206,19 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" t="s">
         <v>79</v>
       </c>
-      <c r="F16" t="s">
-        <v>80</v>
-      </c>
       <c r="H16" t="s">
-        <v>81</v>
-      </c>
-      <c r="I16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1020,40 +1228,82 @@
       <c r="C17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D18" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D20" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D21" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1063,8 +1313,17 @@
       <c r="C22" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -1074,13 +1333,31 @@
       <c r="D23" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -1090,80 +1367,170 @@
       <c r="C25" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B27" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" t="s">
+        <v>55</v>
+      </c>
+      <c r="G28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D29" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B31" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" t="s">
+        <v>55</v>
+      </c>
+      <c r="G31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B32" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B33" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B34" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" t="s">
+        <v>90</v>
+      </c>
+      <c r="G34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -1173,40 +1540,85 @@
       <c r="D35" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" t="s">
+        <v>55</v>
+      </c>
+      <c r="G35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B36" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" t="s">
+        <v>55</v>
+      </c>
+      <c r="G36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B37" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" t="s">
+        <v>55</v>
+      </c>
+      <c r="G37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D38" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" t="s">
+        <v>54</v>
+      </c>
+      <c r="G38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D39" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" t="s">
+        <v>55</v>
+      </c>
+      <c r="G39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>43</v>
       </c>
@@ -1216,48 +1628,102 @@
       <c r="D40" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>55</v>
+      </c>
+      <c r="F40" t="s">
+        <v>55</v>
+      </c>
+      <c r="G40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B41" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41" t="s">
+        <v>93</v>
+      </c>
+      <c r="H41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B42" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>95</v>
+      </c>
+      <c r="F42" t="s">
+        <v>96</v>
+      </c>
+      <c r="G42" t="s">
+        <v>94</v>
+      </c>
+      <c r="H42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B43" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>55</v>
+      </c>
+      <c r="F43" t="s">
+        <v>55</v>
+      </c>
+      <c r="G43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B44" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" t="s">
+        <v>55</v>
+      </c>
+      <c r="G44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B45" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>98</v>
+      </c>
+      <c r="F45" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>49</v>
       </c>
@@ -1267,8 +1733,17 @@
       <c r="C46" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>55</v>
+      </c>
+      <c r="F46" t="s">
+        <v>55</v>
+      </c>
+      <c r="G46" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>50</v>
       </c>
@@ -1278,13 +1753,231 @@
       <c r="D47" t="s">
         <v>0</v>
       </c>
+      <c r="E47" t="s">
+        <v>99</v>
+      </c>
+      <c r="F47" t="s">
+        <v>54</v>
+      </c>
+      <c r="H47" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H47" xr:uid="{33F54A0A-7356-4233-8B23-6276772EBF40}">
+    <filterColumn colId="7">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E888052C-A1E4-4170-B448-65FC7AA7D02E}">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15:E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="L1" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" t="s">
+        <v>117</v>
+      </c>
+      <c r="L3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" t="s">
+        <v>118</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D1869A-68D0-4E7E-BFDA-1868EE10C716}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>